<commit_message>
Adding hyperlinks to Vcycle process script
</commit_message>
<xml_diff>
--- a/Design_Documentation/V_Cycle Process Script.xlsx
+++ b/Design_Documentation/V_Cycle Process Script.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\uidn8311\Desktop\Versions\V-Cycle Process\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\uidn8311\Desktop\window_lifter\Design_Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="7890" yWindow="3180" windowWidth="15015" windowHeight="9330" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="7890" yWindow="3180" windowWidth="15015" windowHeight="9330" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="V-Cycle" sheetId="2" r:id="rId1"/>
@@ -545,6 +545,9 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -554,9 +557,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2025,8 +2025,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:E33"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2090,102 +2090,102 @@
       </c>
     </row>
     <row r="14" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C14" s="53">
+      <c r="C14" s="56">
         <v>1</v>
       </c>
-      <c r="D14" s="54" t="s">
+      <c r="D14" s="57" t="s">
         <v>19</v>
       </c>
-      <c r="E14" s="56" t="s">
+      <c r="E14" s="53" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="15" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C15" s="53"/>
-      <c r="D15" s="54"/>
+      <c r="C15" s="56"/>
+      <c r="D15" s="57"/>
       <c r="E15" s="27" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="16" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C16" s="53"/>
-      <c r="D16" s="54"/>
-      <c r="E16" s="57" t="s">
+      <c r="C16" s="56"/>
+      <c r="D16" s="57"/>
+      <c r="E16" s="54" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="17" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C17" s="53"/>
-      <c r="D17" s="54"/>
-      <c r="E17" s="58" t="s">
+      <c r="C17" s="56"/>
+      <c r="D17" s="57"/>
+      <c r="E17" s="55" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="18" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C18" s="53">
+      <c r="C18" s="56">
         <v>2</v>
       </c>
-      <c r="D18" s="54" t="s">
+      <c r="D18" s="57" t="s">
         <v>21</v>
       </c>
-      <c r="E18" s="56" t="s">
+      <c r="E18" s="53" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="19" spans="3:5" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C19" s="53"/>
-      <c r="D19" s="54"/>
+      <c r="C19" s="56"/>
+      <c r="D19" s="57"/>
       <c r="E19" s="50" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="20" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C20" s="53"/>
-      <c r="D20" s="54"/>
+      <c r="C20" s="56"/>
+      <c r="D20" s="57"/>
       <c r="E20" s="13" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="21" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C21" s="53"/>
-      <c r="D21" s="54"/>
+      <c r="C21" s="56"/>
+      <c r="D21" s="57"/>
       <c r="E21" s="27" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="22" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C22" s="53"/>
-      <c r="D22" s="54"/>
+      <c r="C22" s="56"/>
+      <c r="D22" s="57"/>
       <c r="E22" s="4"/>
     </row>
     <row r="23" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C23" s="53">
+      <c r="C23" s="56">
         <v>3</v>
       </c>
-      <c r="D23" s="54" t="s">
+      <c r="D23" s="57" t="s">
         <v>9</v>
       </c>
-      <c r="E23" s="56" t="s">
+      <c r="E23" s="53" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="24" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C24" s="53"/>
-      <c r="D24" s="54"/>
+      <c r="C24" s="56"/>
+      <c r="D24" s="57"/>
       <c r="E24" s="50" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="25" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C25" s="53"/>
-      <c r="D25" s="54"/>
+      <c r="C25" s="56"/>
+      <c r="D25" s="57"/>
       <c r="E25" s="27" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="26" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C26" s="53"/>
-      <c r="D26" s="54"/>
+      <c r="C26" s="56"/>
+      <c r="D26" s="57"/>
       <c r="E26" s="24" t="s">
         <v>23</v>
       </c>
@@ -2321,10 +2321,10 @@
       </c>
     </row>
     <row r="15" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C15" s="53">
+      <c r="C15" s="56">
         <v>1</v>
       </c>
-      <c r="D15" s="54" t="s">
+      <c r="D15" s="57" t="s">
         <v>13</v>
       </c>
       <c r="E15" s="22" t="s">
@@ -2332,31 +2332,31 @@
       </c>
     </row>
     <row r="16" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C16" s="53"/>
-      <c r="D16" s="54"/>
+      <c r="C16" s="56"/>
+      <c r="D16" s="57"/>
       <c r="E16" s="27" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="17" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C17" s="53"/>
-      <c r="D17" s="54"/>
+      <c r="C17" s="56"/>
+      <c r="D17" s="57"/>
       <c r="E17" s="28" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="18" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C18" s="53"/>
-      <c r="D18" s="54"/>
+      <c r="C18" s="56"/>
+      <c r="D18" s="57"/>
       <c r="E18" s="24" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="19" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C19" s="53">
+      <c r="C19" s="56">
         <v>2</v>
       </c>
-      <c r="D19" s="54" t="s">
+      <c r="D19" s="57" t="s">
         <v>88</v>
       </c>
       <c r="E19" s="22" t="s">
@@ -2364,20 +2364,20 @@
       </c>
     </row>
     <row r="20" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C20" s="53"/>
-      <c r="D20" s="54"/>
+      <c r="C20" s="56"/>
+      <c r="D20" s="57"/>
       <c r="E20" s="28" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="21" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C21" s="53"/>
-      <c r="D21" s="54"/>
+      <c r="C21" s="56"/>
+      <c r="D21" s="57"/>
       <c r="E21" s="7"/>
     </row>
     <row r="22" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C22" s="53"/>
-      <c r="D22" s="54"/>
+      <c r="C22" s="56"/>
+      <c r="D22" s="57"/>
       <c r="E22" s="4"/>
     </row>
     <row r="24" spans="3:5" x14ac:dyDescent="0.25">
@@ -2500,10 +2500,10 @@
       </c>
     </row>
     <row r="15" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C15" s="53">
+      <c r="C15" s="56">
         <v>1</v>
       </c>
-      <c r="D15" s="54" t="s">
+      <c r="D15" s="57" t="s">
         <v>34</v>
       </c>
       <c r="E15" s="22" t="s">
@@ -2511,29 +2511,29 @@
       </c>
     </row>
     <row r="16" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C16" s="53"/>
-      <c r="D16" s="54"/>
+      <c r="C16" s="56"/>
+      <c r="D16" s="57"/>
       <c r="E16" s="27" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="17" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C17" s="53"/>
-      <c r="D17" s="54"/>
+      <c r="C17" s="56"/>
+      <c r="D17" s="57"/>
       <c r="E17" s="28" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="18" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C18" s="53"/>
-      <c r="D18" s="54"/>
+      <c r="C18" s="56"/>
+      <c r="D18" s="57"/>
       <c r="E18" s="29"/>
     </row>
     <row r="19" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C19" s="53">
+      <c r="C19" s="56">
         <v>2</v>
       </c>
-      <c r="D19" s="54" t="s">
+      <c r="D19" s="57" t="s">
         <v>37</v>
       </c>
       <c r="E19" s="34" t="s">
@@ -2541,29 +2541,29 @@
       </c>
     </row>
     <row r="20" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C20" s="53"/>
-      <c r="D20" s="54"/>
+      <c r="C20" s="56"/>
+      <c r="D20" s="57"/>
       <c r="E20" s="27" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="21" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C21" s="53"/>
-      <c r="D21" s="54"/>
+      <c r="C21" s="56"/>
+      <c r="D21" s="57"/>
       <c r="E21" s="27" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="22" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C22" s="53"/>
-      <c r="D22" s="54"/>
+      <c r="C22" s="56"/>
+      <c r="D22" s="57"/>
       <c r="E22" s="24"/>
     </row>
     <row r="23" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C23" s="53">
+      <c r="C23" s="56">
         <v>3</v>
       </c>
-      <c r="D23" s="54" t="s">
+      <c r="D23" s="57" t="s">
         <v>39</v>
       </c>
       <c r="E23" s="34" t="s">
@@ -2571,22 +2571,22 @@
       </c>
     </row>
     <row r="24" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C24" s="53"/>
-      <c r="D24" s="54"/>
+      <c r="C24" s="56"/>
+      <c r="D24" s="57"/>
       <c r="E24" s="34" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="25" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C25" s="53"/>
-      <c r="D25" s="54"/>
+      <c r="C25" s="56"/>
+      <c r="D25" s="57"/>
       <c r="E25" s="27" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="26" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C26" s="53"/>
-      <c r="D26" s="54"/>
+      <c r="C26" s="56"/>
+      <c r="D26" s="57"/>
       <c r="E26" s="24"/>
     </row>
     <row r="28" spans="3:5" x14ac:dyDescent="0.25">
@@ -2702,10 +2702,10 @@
       </c>
     </row>
     <row r="13" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C13" s="53">
+      <c r="C13" s="56">
         <v>1</v>
       </c>
-      <c r="D13" s="54" t="s">
+      <c r="D13" s="57" t="s">
         <v>48</v>
       </c>
       <c r="E13" s="35" t="s">
@@ -2713,29 +2713,29 @@
       </c>
     </row>
     <row r="14" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C14" s="53"/>
-      <c r="D14" s="54"/>
+      <c r="C14" s="56"/>
+      <c r="D14" s="57"/>
       <c r="E14" s="39" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="15" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C15" s="53"/>
-      <c r="D15" s="54"/>
+      <c r="C15" s="56"/>
+      <c r="D15" s="57"/>
       <c r="E15" s="28" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="16" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C16" s="53"/>
-      <c r="D16" s="54"/>
+      <c r="C16" s="56"/>
+      <c r="D16" s="57"/>
       <c r="E16" s="29"/>
     </row>
     <row r="17" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C17" s="53">
+      <c r="C17" s="56">
         <v>2</v>
       </c>
-      <c r="D17" s="54" t="s">
+      <c r="D17" s="57" t="s">
         <v>47</v>
       </c>
       <c r="E17" s="35" t="s">
@@ -2743,22 +2743,22 @@
       </c>
     </row>
     <row r="18" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C18" s="53"/>
-      <c r="D18" s="54"/>
+      <c r="C18" s="56"/>
+      <c r="D18" s="57"/>
       <c r="E18" s="27" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="19" spans="3:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="C19" s="53"/>
-      <c r="D19" s="54"/>
+      <c r="C19" s="56"/>
+      <c r="D19" s="57"/>
       <c r="E19" s="38" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="20" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C20" s="53"/>
-      <c r="D20" s="54"/>
+      <c r="C20" s="56"/>
+      <c r="D20" s="57"/>
       <c r="E20" s="29"/>
     </row>
     <row r="22" spans="3:5" x14ac:dyDescent="0.25">
@@ -2869,10 +2869,10 @@
       </c>
     </row>
     <row r="13" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C13" s="53">
+      <c r="C13" s="56">
         <v>1</v>
       </c>
-      <c r="D13" s="54" t="s">
+      <c r="D13" s="57" t="s">
         <v>48</v>
       </c>
       <c r="E13" s="35" t="s">
@@ -2880,29 +2880,29 @@
       </c>
     </row>
     <row r="14" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C14" s="53"/>
-      <c r="D14" s="54"/>
+      <c r="C14" s="56"/>
+      <c r="D14" s="57"/>
       <c r="E14" s="39" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="15" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C15" s="53"/>
-      <c r="D15" s="54"/>
+      <c r="C15" s="56"/>
+      <c r="D15" s="57"/>
       <c r="E15" s="28" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="16" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C16" s="53"/>
-      <c r="D16" s="54"/>
+      <c r="C16" s="56"/>
+      <c r="D16" s="57"/>
       <c r="E16" s="29"/>
     </row>
     <row r="17" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C17" s="53">
+      <c r="C17" s="56">
         <v>2</v>
       </c>
-      <c r="D17" s="54" t="s">
+      <c r="D17" s="57" t="s">
         <v>47</v>
       </c>
       <c r="E17" s="35" t="s">
@@ -2910,22 +2910,22 @@
       </c>
     </row>
     <row r="18" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C18" s="53"/>
-      <c r="D18" s="54"/>
+      <c r="C18" s="56"/>
+      <c r="D18" s="57"/>
       <c r="E18" s="27" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="19" spans="3:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="C19" s="53"/>
-      <c r="D19" s="54"/>
+      <c r="C19" s="56"/>
+      <c r="D19" s="57"/>
       <c r="E19" s="38" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="20" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C20" s="53"/>
-      <c r="D20" s="54"/>
+      <c r="C20" s="56"/>
+      <c r="D20" s="57"/>
       <c r="E20" s="29"/>
     </row>
     <row r="23" spans="3:5" x14ac:dyDescent="0.25">
@@ -2964,8 +2964,8 @@
       <c r="D28" s="36"/>
     </row>
     <row r="29" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C29" s="55"/>
-      <c r="D29" s="54" t="s">
+      <c r="C29" s="58"/>
+      <c r="D29" s="57" t="s">
         <v>85</v>
       </c>
       <c r="E29" s="35" t="s">
@@ -2973,22 +2973,22 @@
       </c>
     </row>
     <row r="30" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C30" s="55"/>
-      <c r="D30" s="54"/>
+      <c r="C30" s="58"/>
+      <c r="D30" s="57"/>
       <c r="E30" s="27" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="31" spans="3:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="C31" s="55"/>
-      <c r="D31" s="54"/>
+      <c r="C31" s="58"/>
+      <c r="D31" s="57"/>
       <c r="E31" s="38" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="32" spans="3:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="C32" s="55"/>
-      <c r="D32" s="54"/>
+      <c r="C32" s="58"/>
+      <c r="D32" s="57"/>
       <c r="E32" s="37" t="s">
         <v>86</v>
       </c>

</xml_diff>